<commit_message>
added dummy L2S2 system
</commit_message>
<xml_diff>
--- a/Nutritional_info.xlsx
+++ b/Nutritional_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/GM1_G3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7B88D6-636A-4E40-8AD4-FD00AA9530E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7111D82F-15CF-634F-A617-A4CCADDF6FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="8180" windowWidth="28040" windowHeight="16480" xr2:uid="{033E848B-DD3C-CD40-A057-616C66D08716}"/>
+    <workbookView xWindow="160" yWindow="1920" windowWidth="28040" windowHeight="16480" xr2:uid="{033E848B-DD3C-CD40-A057-616C66D08716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>